<commit_message>
add testcase boundary and equivalence
</commit_message>
<xml_diff>
--- a/Selenium_Test_C#/bin/Debug/Testcase_Grade.xlsx
+++ b/Selenium_Test_C#/bin/Debug/Testcase_Grade.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SWTesting_Proj3_Selenium_Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SWTesting_Proj3_Selenium_Test\Selenium_Test_C#\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="37">
   <si>
     <t>Midtern</t>
   </si>
@@ -64,6 +64,72 @@
   </si>
   <si>
     <t>Average grade: 85.6(B)</t>
+  </si>
+  <si>
+    <t>Course</t>
+  </si>
+  <si>
+    <t>Average grade: 98.0 (A+)</t>
+  </si>
+  <si>
+    <t>Average grade: 96.0 (A)</t>
+  </si>
+  <si>
+    <t>Average grade: 90.0 (A-)</t>
+  </si>
+  <si>
+    <t>Average grade: 89.0 (B+)</t>
+  </si>
+  <si>
+    <t>Average grade: 85.0 (B)</t>
+  </si>
+  <si>
+    <t>Average grade: 81.0 (B-)</t>
+  </si>
+  <si>
+    <t>Average grade: 78.0 (C+)</t>
+  </si>
+  <si>
+    <t>Average grade: 74.0 (C)</t>
+  </si>
+  <si>
+    <t>Average grade: 72.0 (C-)</t>
+  </si>
+  <si>
+    <t>Average grade: 67.0 (D+)</t>
+  </si>
+  <si>
+    <t>Average grade: 65.0 (D)</t>
+  </si>
+  <si>
+    <t>Average grade: 61.0 (D-)</t>
+  </si>
+  <si>
+    <t>Average grade: 55.0 (F)</t>
+  </si>
+  <si>
+    <t>Average grade: F (0.00)</t>
+  </si>
+  <si>
+    <t>Average grade: D (1.00)</t>
+  </si>
+  <si>
+    <t>Average grade: 50.0 (F)</t>
+  </si>
+  <si>
+    <t>Average grade: 99.0 (A+)</t>
+  </si>
+  <si>
+    <t>Average grade: 100.0 (A+)</t>
+  </si>
+  <si>
+    <t>Average grade: 101.0</t>
+  </si>
+  <si>
+    <t>Please provide positive weight for the Assignments/Exams.</t>
+  </si>
+  <si>
+    <t>This result is based on a total weight of 102%. Please make sure that the weight inputs are correct.</t>
   </si>
 </sst>
 </file>
@@ -553,14 +619,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -889,18 +951,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G78"/>
+  <dimension ref="A1:G105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="F77" sqref="F77"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F106" sqref="F106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="8.7265625" style="1"/>
-    <col min="5" max="5" width="26.90625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="28.81640625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="25.453125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="29.08984375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="28.81640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="25.453125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -938,13 +1000,13 @@
       <c r="D3">
         <v>80</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -983,13 +1045,13 @@
       <c r="D6">
         <v>80</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1028,10 +1090,10 @@
       <c r="D9">
         <v>80</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1070,10 +1132,10 @@
       <c r="D12">
         <v>80</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1112,10 +1174,10 @@
       <c r="D15">
         <v>80</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1154,10 +1216,10 @@
       <c r="D18">
         <v>80</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1196,10 +1258,10 @@
       <c r="D21">
         <v>80</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F21" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1238,10 +1300,10 @@
       <c r="D24">
         <v>60</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F24" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1280,7 +1342,7 @@
       <c r="D27">
         <v>80</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1319,7 +1381,7 @@
       <c r="D30">
         <v>60</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1358,7 +1420,7 @@
       <c r="D33">
         <v>80</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="E33" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1397,7 +1459,7 @@
       <c r="D36">
         <v>60</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="E36" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1436,10 +1498,10 @@
       <c r="D39">
         <v>80</v>
       </c>
-      <c r="E39" s="4" t="s">
+      <c r="E39" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F39" s="4" t="s">
+      <c r="F39" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1478,10 +1540,10 @@
       <c r="D42">
         <v>80</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="E42" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F42" s="4" t="s">
+      <c r="F42" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1520,7 +1582,7 @@
       <c r="D45">
         <v>80</v>
       </c>
-      <c r="E45" s="4" t="s">
+      <c r="E45" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1559,7 +1621,7 @@
       <c r="D48">
         <v>80</v>
       </c>
-      <c r="E48" s="4" t="s">
+      <c r="E48" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1598,7 +1660,7 @@
       <c r="D51">
         <v>80</v>
       </c>
-      <c r="E51" s="4" t="s">
+      <c r="E51" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1637,7 +1699,7 @@
       <c r="D54">
         <v>80</v>
       </c>
-      <c r="E54" s="4" t="s">
+      <c r="E54" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1676,7 +1738,7 @@
       <c r="D57">
         <v>80</v>
       </c>
-      <c r="E57" s="4" t="s">
+      <c r="E57" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1715,7 +1777,7 @@
       <c r="D60">
         <v>60</v>
       </c>
-      <c r="E60" s="4" t="s">
+      <c r="E60" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1754,10 +1816,10 @@
       <c r="D63">
         <v>80</v>
       </c>
-      <c r="E63" s="4" t="s">
+      <c r="E63" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F63" s="4" t="s">
+      <c r="F63" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1771,7 +1833,7 @@
       <c r="D64">
         <v>0</v>
       </c>
-      <c r="E64" s="3"/>
+      <c r="E64" s="2"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B65" t="s">
@@ -1784,7 +1846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="38.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>22</v>
       </c>
@@ -1797,7 +1859,7 @@
       <c r="D66">
         <v>0</v>
       </c>
-      <c r="E66" s="3" t="s">
+      <c r="E66" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1875,10 +1937,10 @@
       <c r="D72">
         <v>80</v>
       </c>
-      <c r="E72" s="4" t="s">
+      <c r="E72" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F72" s="4" t="s">
+      <c r="F72" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1904,7 +1966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="38.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>25</v>
       </c>
@@ -1917,7 +1979,7 @@
       <c r="D75">
         <v>0</v>
       </c>
-      <c r="E75" s="3" t="s">
+      <c r="E75" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1956,8 +2018,470 @@
       <c r="D78">
         <v>50</v>
       </c>
-      <c r="E78" s="4" t="s">
+      <c r="E78" s="2" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A79">
+        <v>27</v>
+      </c>
+      <c r="B79" t="s">
+        <v>15</v>
+      </c>
+      <c r="C79" s="1">
+        <v>55</v>
+      </c>
+      <c r="D79">
+        <v>40</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A80">
+        <v>28</v>
+      </c>
+      <c r="B80" t="s">
+        <v>15</v>
+      </c>
+      <c r="C80" s="1">
+        <v>61</v>
+      </c>
+      <c r="D80">
+        <v>40</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A81">
+        <v>29</v>
+      </c>
+      <c r="B81" t="s">
+        <v>15</v>
+      </c>
+      <c r="C81" s="1">
+        <v>65</v>
+      </c>
+      <c r="D81">
+        <v>40</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A82">
+        <v>30</v>
+      </c>
+      <c r="B82" t="s">
+        <v>15</v>
+      </c>
+      <c r="C82" s="1">
+        <v>67</v>
+      </c>
+      <c r="D82">
+        <v>40</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A83">
+        <v>31</v>
+      </c>
+      <c r="B83" t="s">
+        <v>15</v>
+      </c>
+      <c r="C83" s="1">
+        <v>72</v>
+      </c>
+      <c r="D83">
+        <v>40</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A84">
+        <v>32</v>
+      </c>
+      <c r="B84" t="s">
+        <v>15</v>
+      </c>
+      <c r="C84" s="1">
+        <v>74</v>
+      </c>
+      <c r="D84">
+        <v>40</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A85">
+        <v>33</v>
+      </c>
+      <c r="B85" t="s">
+        <v>15</v>
+      </c>
+      <c r="C85" s="1">
+        <v>78</v>
+      </c>
+      <c r="D85">
+        <v>40</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A86">
+        <v>34</v>
+      </c>
+      <c r="B86" t="s">
+        <v>15</v>
+      </c>
+      <c r="C86" s="1">
+        <v>81</v>
+      </c>
+      <c r="D86">
+        <v>40</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A87">
+        <v>35</v>
+      </c>
+      <c r="B87" t="s">
+        <v>15</v>
+      </c>
+      <c r="C87" s="1">
+        <v>85</v>
+      </c>
+      <c r="D87">
+        <v>40</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A88">
+        <v>36</v>
+      </c>
+      <c r="B88" t="s">
+        <v>15</v>
+      </c>
+      <c r="C88" s="1">
+        <v>89</v>
+      </c>
+      <c r="D88">
+        <v>40</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A89">
+        <v>37</v>
+      </c>
+      <c r="B89" t="s">
+        <v>15</v>
+      </c>
+      <c r="C89" s="1">
+        <v>90</v>
+      </c>
+      <c r="D89">
+        <v>100</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A90">
+        <v>38</v>
+      </c>
+      <c r="B90" t="s">
+        <v>15</v>
+      </c>
+      <c r="C90" s="1">
+        <v>96</v>
+      </c>
+      <c r="D90">
+        <v>101</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A91">
+        <v>39</v>
+      </c>
+      <c r="B91" t="s">
+        <v>15</v>
+      </c>
+      <c r="C91" s="1">
+        <v>98</v>
+      </c>
+      <c r="D91">
+        <v>101</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="25" x14ac:dyDescent="0.35">
+      <c r="A92">
+        <v>40</v>
+      </c>
+      <c r="B92" t="s">
+        <v>15</v>
+      </c>
+      <c r="C92" s="1">
+        <v>-1</v>
+      </c>
+      <c r="D92">
+        <v>50</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A93">
+        <v>41</v>
+      </c>
+      <c r="B93" t="s">
+        <v>15</v>
+      </c>
+      <c r="C93" s="1">
+        <v>0</v>
+      </c>
+      <c r="D93">
+        <v>50</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A94">
+        <v>42</v>
+      </c>
+      <c r="B94" t="s">
+        <v>15</v>
+      </c>
+      <c r="C94" s="1">
+        <v>1</v>
+      </c>
+      <c r="D94">
+        <v>50</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A95">
+        <v>43</v>
+      </c>
+      <c r="B95" t="s">
+        <v>15</v>
+      </c>
+      <c r="C95" s="1">
+        <v>50</v>
+      </c>
+      <c r="D95">
+        <v>50</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A96">
+        <v>44</v>
+      </c>
+      <c r="B96" t="s">
+        <v>15</v>
+      </c>
+      <c r="C96" s="1">
+        <v>99</v>
+      </c>
+      <c r="D96">
+        <v>50</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A97">
+        <v>45</v>
+      </c>
+      <c r="B97" t="s">
+        <v>15</v>
+      </c>
+      <c r="C97" s="1">
+        <v>100</v>
+      </c>
+      <c r="D97">
+        <v>50</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A98">
+        <v>46</v>
+      </c>
+      <c r="B98" t="s">
+        <v>15</v>
+      </c>
+      <c r="C98" s="1">
+        <v>101</v>
+      </c>
+      <c r="D98">
+        <v>50</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="25" x14ac:dyDescent="0.35">
+      <c r="A99">
+        <v>47</v>
+      </c>
+      <c r="B99" t="s">
+        <v>15</v>
+      </c>
+      <c r="C99" s="1">
+        <v>50</v>
+      </c>
+      <c r="D99">
+        <v>-1</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="25" x14ac:dyDescent="0.35">
+      <c r="A100">
+        <v>48</v>
+      </c>
+      <c r="B100" t="s">
+        <v>15</v>
+      </c>
+      <c r="C100" s="1">
+        <v>50</v>
+      </c>
+      <c r="D100">
+        <v>0</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A101">
+        <v>49</v>
+      </c>
+      <c r="B101" t="s">
+        <v>15</v>
+      </c>
+      <c r="C101" s="1">
+        <v>50</v>
+      </c>
+      <c r="D101">
+        <v>1</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A102">
+        <v>50</v>
+      </c>
+      <c r="B102" t="s">
+        <v>15</v>
+      </c>
+      <c r="C102" s="1">
+        <v>50</v>
+      </c>
+      <c r="D102">
+        <v>50</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A103">
+        <v>51</v>
+      </c>
+      <c r="B103" t="s">
+        <v>15</v>
+      </c>
+      <c r="C103" s="1">
+        <v>50</v>
+      </c>
+      <c r="D103">
+        <v>100</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A104">
+        <v>52</v>
+      </c>
+      <c r="B104" t="s">
+        <v>15</v>
+      </c>
+      <c r="C104" s="1">
+        <v>50</v>
+      </c>
+      <c r="D104">
+        <v>101</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" ht="50" x14ac:dyDescent="0.35">
+      <c r="A105">
+        <v>53</v>
+      </c>
+      <c r="B105" t="s">
+        <v>15</v>
+      </c>
+      <c r="C105" s="1">
+        <v>50</v>
+      </c>
+      <c r="D105">
+        <v>102</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
complete grade cat test
</commit_message>
<xml_diff>
--- a/Selenium_Test_C#/bin/Debug/Testcase_Grade.xlsx
+++ b/Selenium_Test_C#/bin/Debug/Testcase_Grade.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="35">
   <si>
     <t>Midtern</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Please provide a valid grade for item #1.</t>
   </si>
   <si>
-    <t>The grade cannot be a mixture of letter and a grading system that has more than 100 points..</t>
-  </si>
-  <si>
     <t>Please provide a valid weight for item #1.</t>
   </si>
   <si>
@@ -54,18 +51,6 @@
     <t>Average grade: A- (3.50)</t>
   </si>
   <si>
-    <t>Print: Please provide positive weight for the Assignments/Exams.</t>
-  </si>
-  <si>
-    <t>Print: Average grade: B+ (3.40)</t>
-  </si>
-  <si>
-    <t>Average grade: 87.5(B+)</t>
-  </si>
-  <si>
-    <t>Average grade: 85.6(B)</t>
-  </si>
-  <si>
     <t>Course</t>
   </si>
   <si>
@@ -130,6 +115,15 @@
   </si>
   <si>
     <t>This result is based on a total weight of 102%. Please make sure that the weight inputs are correct.</t>
+  </si>
+  <si>
+    <t>Average grade: B+ (3.40)</t>
+  </si>
+  <si>
+    <t>Average grade: 87.5 (B+)</t>
+  </si>
+  <si>
+    <t>Average grade: 85.6 (B)</t>
   </si>
 </sst>
 </file>
@@ -953,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F106" sqref="F106"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="F75" sqref="F75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1001,13 +995,13 @@
         <v>80</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -1046,13 +1040,13 @@
         <v>80</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -1091,7 +1085,7 @@
         <v>80</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>5</v>
@@ -1133,7 +1127,7 @@
         <v>80</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>5</v>
@@ -1175,7 +1169,7 @@
         <v>80</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>5</v>
@@ -1217,7 +1211,7 @@
         <v>80</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>5</v>
@@ -1262,7 +1256,7 @@
         <v>5</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
@@ -1304,7 +1298,7 @@
         <v>5</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
@@ -1499,10 +1493,10 @@
         <v>80</v>
       </c>
       <c r="E39" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F39" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
@@ -1541,10 +1535,10 @@
         <v>80</v>
       </c>
       <c r="E42" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F42" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
@@ -1583,7 +1577,7 @@
         <v>80</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
@@ -1622,7 +1616,7 @@
         <v>80</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
@@ -1661,7 +1655,7 @@
         <v>80</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
@@ -1700,7 +1694,7 @@
         <v>80</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.35">
@@ -1739,7 +1733,7 @@
         <v>80</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
@@ -1778,7 +1772,7 @@
         <v>60</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.35">
@@ -1817,10 +1811,10 @@
         <v>80</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.35">
@@ -1846,7 +1840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" ht="25" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>22</v>
       </c>
@@ -1860,7 +1854,7 @@
         <v>0</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.35">
@@ -1899,7 +1893,7 @@
         <v>60</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.35">
@@ -1938,10 +1932,10 @@
         <v>80</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.35">
@@ -1966,7 +1960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" ht="25" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>25</v>
       </c>
@@ -1980,7 +1974,7 @@
         <v>0</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.35">
@@ -2019,7 +2013,7 @@
         <v>50</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.35">
@@ -2027,7 +2021,7 @@
         <v>27</v>
       </c>
       <c r="B79" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C79" s="1">
         <v>55</v>
@@ -2036,7 +2030,7 @@
         <v>40</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.35">
@@ -2044,7 +2038,7 @@
         <v>28</v>
       </c>
       <c r="B80" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C80" s="1">
         <v>61</v>
@@ -2053,7 +2047,7 @@
         <v>40</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.35">
@@ -2061,7 +2055,7 @@
         <v>29</v>
       </c>
       <c r="B81" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C81" s="1">
         <v>65</v>
@@ -2070,7 +2064,7 @@
         <v>40</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
@@ -2078,7 +2072,7 @@
         <v>30</v>
       </c>
       <c r="B82" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C82" s="1">
         <v>67</v>
@@ -2087,7 +2081,7 @@
         <v>40</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.35">
@@ -2095,7 +2089,7 @@
         <v>31</v>
       </c>
       <c r="B83" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C83" s="1">
         <v>72</v>
@@ -2104,7 +2098,7 @@
         <v>40</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.35">
@@ -2112,7 +2106,7 @@
         <v>32</v>
       </c>
       <c r="B84" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C84" s="1">
         <v>74</v>
@@ -2121,7 +2115,7 @@
         <v>40</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.35">
@@ -2129,7 +2123,7 @@
         <v>33</v>
       </c>
       <c r="B85" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C85" s="1">
         <v>78</v>
@@ -2138,7 +2132,7 @@
         <v>40</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.35">
@@ -2146,7 +2140,7 @@
         <v>34</v>
       </c>
       <c r="B86" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C86" s="1">
         <v>81</v>
@@ -2155,7 +2149,7 @@
         <v>40</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.35">
@@ -2163,7 +2157,7 @@
         <v>35</v>
       </c>
       <c r="B87" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C87" s="1">
         <v>85</v>
@@ -2172,7 +2166,7 @@
         <v>40</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.35">
@@ -2180,7 +2174,7 @@
         <v>36</v>
       </c>
       <c r="B88" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C88" s="1">
         <v>89</v>
@@ -2189,7 +2183,7 @@
         <v>40</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.35">
@@ -2197,7 +2191,7 @@
         <v>37</v>
       </c>
       <c r="B89" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C89" s="1">
         <v>90</v>
@@ -2206,7 +2200,7 @@
         <v>100</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.35">
@@ -2214,7 +2208,7 @@
         <v>38</v>
       </c>
       <c r="B90" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C90" s="1">
         <v>96</v>
@@ -2223,7 +2217,7 @@
         <v>101</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.35">
@@ -2231,7 +2225,7 @@
         <v>39</v>
       </c>
       <c r="B91" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C91" s="1">
         <v>98</v>
@@ -2240,7 +2234,7 @@
         <v>101</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="25" x14ac:dyDescent="0.35">
@@ -2248,7 +2242,7 @@
         <v>40</v>
       </c>
       <c r="B92" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C92" s="1">
         <v>-1</v>
@@ -2265,7 +2259,7 @@
         <v>41</v>
       </c>
       <c r="B93" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C93" s="1">
         <v>0</v>
@@ -2274,7 +2268,7 @@
         <v>50</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.35">
@@ -2282,7 +2276,7 @@
         <v>42</v>
       </c>
       <c r="B94" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C94" s="1">
         <v>1</v>
@@ -2291,7 +2285,7 @@
         <v>50</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.35">
@@ -2299,7 +2293,7 @@
         <v>43</v>
       </c>
       <c r="B95" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C95" s="1">
         <v>50</v>
@@ -2308,7 +2302,7 @@
         <v>50</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.35">
@@ -2316,7 +2310,7 @@
         <v>44</v>
       </c>
       <c r="B96" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C96" s="1">
         <v>99</v>
@@ -2325,7 +2319,7 @@
         <v>50</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.35">
@@ -2333,7 +2327,7 @@
         <v>45</v>
       </c>
       <c r="B97" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C97" s="1">
         <v>100</v>
@@ -2342,7 +2336,7 @@
         <v>50</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.35">
@@ -2350,7 +2344,7 @@
         <v>46</v>
       </c>
       <c r="B98" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C98" s="1">
         <v>101</v>
@@ -2359,7 +2353,7 @@
         <v>50</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="25" x14ac:dyDescent="0.35">
@@ -2367,7 +2361,7 @@
         <v>47</v>
       </c>
       <c r="B99" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C99" s="1">
         <v>50</v>
@@ -2376,7 +2370,7 @@
         <v>-1</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="100" spans="1:6" ht="25" x14ac:dyDescent="0.35">
@@ -2384,7 +2378,7 @@
         <v>48</v>
       </c>
       <c r="B100" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C100" s="1">
         <v>50</v>
@@ -2393,7 +2387,7 @@
         <v>0</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.35">
@@ -2401,7 +2395,7 @@
         <v>49</v>
       </c>
       <c r="B101" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C101" s="1">
         <v>50</v>
@@ -2410,7 +2404,7 @@
         <v>1</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.35">
@@ -2418,7 +2412,7 @@
         <v>50</v>
       </c>
       <c r="B102" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C102" s="1">
         <v>50</v>
@@ -2427,7 +2421,7 @@
         <v>50</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.35">
@@ -2435,7 +2429,7 @@
         <v>51</v>
       </c>
       <c r="B103" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C103" s="1">
         <v>50</v>
@@ -2444,7 +2438,7 @@
         <v>100</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.35">
@@ -2452,7 +2446,7 @@
         <v>52</v>
       </c>
       <c r="B104" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C104" s="1">
         <v>50</v>
@@ -2461,7 +2455,7 @@
         <v>101</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="105" spans="1:6" ht="50" x14ac:dyDescent="0.35">
@@ -2469,7 +2463,7 @@
         <v>53</v>
       </c>
       <c r="B105" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C105" s="1">
         <v>50</v>
@@ -2478,10 +2472,10 @@
         <v>102</v>
       </c>
       <c r="E105" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F105" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="F105" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>